<commit_message>
first commit for dev
</commit_message>
<xml_diff>
--- a/data/fakesystem/sys_SSE.xlsx
+++ b/data/fakesystem/sys_SSE.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khor Kean Teng\Downloads\AUP Automata\data\fakesystem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F4256F-E62B-4BBF-B5BA-C80F7C1A8AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="444">
   <si>
     <t>Department</t>
   </si>
@@ -1337,13 +1343,22 @@
   </si>
   <si>
     <t>SSE</t>
+  </si>
+  <si>
+    <t>Disable Flag *</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1368,7 +1383,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1391,13 +1406,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1406,13 +1435,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1450,7 +1487,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1484,6 +1521,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1518,9 +1556,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1693,14 +1732,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F198"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1719,8 +1760,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1739,8 +1783,11 @@
       <c r="F2">
         <v>110773</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1756,8 +1803,11 @@
       <c r="E3" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1773,8 +1823,11 @@
       <c r="E4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1790,8 +1843,11 @@
       <c r="E5" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1807,8 +1863,11 @@
       <c r="E6" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1824,8 +1883,11 @@
       <c r="E7" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1841,8 +1903,11 @@
       <c r="E8" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1858,8 +1923,11 @@
       <c r="E9" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1875,8 +1943,11 @@
       <c r="E10" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1892,8 +1963,11 @@
       <c r="E11" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1909,8 +1983,11 @@
       <c r="E12" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1926,8 +2003,11 @@
       <c r="E13" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1943,8 +2023,11 @@
       <c r="E14" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1960,8 +2043,11 @@
       <c r="E15" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1977,8 +2063,11 @@
       <c r="E16" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1994,8 +2083,11 @@
       <c r="E17" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2011,8 +2103,11 @@
       <c r="E18" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2028,8 +2123,11 @@
       <c r="E19" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2045,8 +2143,11 @@
       <c r="E20" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2062,8 +2163,11 @@
       <c r="E21" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2079,8 +2183,11 @@
       <c r="E22" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -2096,8 +2203,11 @@
       <c r="E23" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="G23" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2113,8 +2223,11 @@
       <c r="E24" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="G24" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2130,8 +2243,11 @@
       <c r="E25" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="G25" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -2147,8 +2263,11 @@
       <c r="E26" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="G26" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2164,8 +2283,11 @@
       <c r="E27" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="G27" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2181,8 +2303,11 @@
       <c r="E28" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="G28" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2198,8 +2323,11 @@
       <c r="E29" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="G29" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2215,8 +2343,11 @@
       <c r="E30" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="G30" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2232,8 +2363,11 @@
       <c r="E31" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="G31" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2249,8 +2383,11 @@
       <c r="E32" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="G32" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -2266,8 +2403,11 @@
       <c r="E33" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="G33" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -2283,8 +2423,11 @@
       <c r="E34" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="G34" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2300,8 +2443,11 @@
       <c r="E35" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="G35" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2317,8 +2463,11 @@
       <c r="E36" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="G36" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -2334,8 +2483,11 @@
       <c r="E37" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="G37" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -2351,8 +2503,11 @@
       <c r="E38" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="G38" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -2368,8 +2523,11 @@
       <c r="E39" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="G39" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -2385,8 +2543,11 @@
       <c r="E40" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="G40" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -2402,8 +2563,11 @@
       <c r="E41" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="G41" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -2419,8 +2583,11 @@
       <c r="E42" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="G42" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -2436,8 +2603,11 @@
       <c r="E43" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="G43" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -2453,8 +2623,11 @@
       <c r="E44" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="G44" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -2470,8 +2643,11 @@
       <c r="E45" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="G45" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -2487,8 +2663,11 @@
       <c r="E46" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="G46" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2504,8 +2683,11 @@
       <c r="E47" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="G47" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2521,8 +2703,11 @@
       <c r="E48" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="G48" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2538,8 +2723,11 @@
       <c r="E49" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="G49" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2555,8 +2743,11 @@
       <c r="E50" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="G50" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2572,8 +2763,11 @@
       <c r="E51" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="G51" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2589,8 +2783,11 @@
       <c r="E52" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="G52" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2606,8 +2803,11 @@
       <c r="E53" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="G53" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2623,8 +2823,11 @@
       <c r="E54" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="G54" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -2640,8 +2843,11 @@
       <c r="E55" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="G55" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -2657,8 +2863,11 @@
       <c r="E56" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="G56" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -2674,8 +2883,11 @@
       <c r="E57" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="G57" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -2691,8 +2903,11 @@
       <c r="E58" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="G58" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -2708,8 +2923,11 @@
       <c r="E59" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="G59" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -2725,8 +2943,11 @@
       <c r="E60" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="G60" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -2742,8 +2963,11 @@
       <c r="E61" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="G61" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -2759,8 +2983,11 @@
       <c r="E62" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="G62" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -2776,8 +3003,11 @@
       <c r="E63" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="G63" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -2793,8 +3023,11 @@
       <c r="E64" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="G64" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -2810,8 +3043,11 @@
       <c r="E65" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="G65" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -2827,8 +3063,11 @@
       <c r="E66" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="G66" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -2844,8 +3083,11 @@
       <c r="E67" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="G67" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -2861,8 +3103,11 @@
       <c r="E68" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="G68" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -2878,8 +3123,11 @@
       <c r="E69" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="G69" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -2895,8 +3143,11 @@
       <c r="E70" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="G70" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -2912,8 +3163,11 @@
       <c r="E71" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="G71" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -2929,8 +3183,11 @@
       <c r="E72" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="G72" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -2946,8 +3203,11 @@
       <c r="E73" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="G73" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -2963,8 +3223,11 @@
       <c r="E74" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="G74" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -2980,8 +3243,11 @@
       <c r="E75" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="G75" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -2997,8 +3263,11 @@
       <c r="E76" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="G76" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -3014,8 +3283,11 @@
       <c r="E77" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="G77" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -3031,8 +3303,11 @@
       <c r="E78" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="G78" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -3048,8 +3323,11 @@
       <c r="E79" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="G79" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -3065,8 +3343,11 @@
       <c r="E80" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="G80" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -3082,8 +3363,11 @@
       <c r="E81" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="G81" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -3099,8 +3383,11 @@
       <c r="E82" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="G82" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -3116,8 +3403,11 @@
       <c r="E83" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="G83" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>14</v>
       </c>
@@ -3133,8 +3423,11 @@
       <c r="E84" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="G84" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>14</v>
       </c>
@@ -3150,8 +3443,11 @@
       <c r="E85" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="G85" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -3167,8 +3463,11 @@
       <c r="E86" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="G86" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -3184,8 +3483,11 @@
       <c r="E87" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="G87" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -3201,8 +3503,11 @@
       <c r="E88" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="G88" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -3218,8 +3523,11 @@
       <c r="E89" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="G89" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -3235,8 +3543,11 @@
       <c r="E90" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="G90" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -3252,8 +3563,11 @@
       <c r="E91" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="G91" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -3269,8 +3583,11 @@
       <c r="E92" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="G92" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -3286,8 +3603,11 @@
       <c r="E93" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="G93" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>15</v>
       </c>
@@ -3303,8 +3623,11 @@
       <c r="E94" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="G94" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -3320,8 +3643,11 @@
       <c r="E95" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="G95" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>15</v>
       </c>
@@ -3337,8 +3663,11 @@
       <c r="E96" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="G96" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>15</v>
       </c>
@@ -3354,8 +3683,11 @@
       <c r="E97" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="G97" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -3371,8 +3703,11 @@
       <c r="E98" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="G98" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>15</v>
       </c>
@@ -3388,8 +3723,11 @@
       <c r="E99" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="G99" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -3405,8 +3743,11 @@
       <c r="E100" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="G100" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -3422,8 +3763,11 @@
       <c r="E101" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="G101" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -3439,8 +3783,11 @@
       <c r="E102" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="G102" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -3456,8 +3803,11 @@
       <c r="E103" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="G103" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -3473,8 +3823,11 @@
       <c r="E104" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="G104" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -3490,8 +3843,11 @@
       <c r="E105" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="G105" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -3507,8 +3863,11 @@
       <c r="E106" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="G106" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -3524,8 +3883,11 @@
       <c r="E107" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="G107" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -3541,8 +3903,11 @@
       <c r="E108" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="G108" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>16</v>
       </c>
@@ -3558,8 +3923,11 @@
       <c r="E109" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="G109" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -3575,8 +3943,11 @@
       <c r="E110" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="G110" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>16</v>
       </c>
@@ -3592,8 +3963,11 @@
       <c r="E111" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="G111" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>17</v>
       </c>
@@ -3609,8 +3983,11 @@
       <c r="E112" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="G112" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>17</v>
       </c>
@@ -3626,8 +4003,11 @@
       <c r="E113" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="G113" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -3643,8 +4023,11 @@
       <c r="E114" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="G114" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>17</v>
       </c>
@@ -3660,8 +4043,11 @@
       <c r="E115" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="G115" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>17</v>
       </c>
@@ -3677,8 +4063,11 @@
       <c r="E116" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="G116" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>17</v>
       </c>
@@ -3694,8 +4083,11 @@
       <c r="E117" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="G117" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>17</v>
       </c>
@@ -3711,8 +4103,11 @@
       <c r="E118" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="G118" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>17</v>
       </c>
@@ -3728,8 +4123,11 @@
       <c r="E119" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="G119" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>18</v>
       </c>
@@ -3745,8 +4143,11 @@
       <c r="E120" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="G120" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>18</v>
       </c>
@@ -3762,8 +4163,11 @@
       <c r="E121" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="G121" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>18</v>
       </c>
@@ -3779,8 +4183,11 @@
       <c r="E122" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="G122" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>18</v>
       </c>
@@ -3796,8 +4203,11 @@
       <c r="E123" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="G123" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -3813,8 +4223,11 @@
       <c r="E124" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="G124" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>18</v>
       </c>
@@ -3830,8 +4243,11 @@
       <c r="E125" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="G125" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>19</v>
       </c>
@@ -3847,8 +4263,11 @@
       <c r="E126" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="G126" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -3864,8 +4283,11 @@
       <c r="E127" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="G127" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>19</v>
       </c>
@@ -3881,8 +4303,11 @@
       <c r="E128" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="G128" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>19</v>
       </c>
@@ -3898,8 +4323,11 @@
       <c r="E129" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="G129" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>19</v>
       </c>
@@ -3915,8 +4343,11 @@
       <c r="E130" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="G130" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>19</v>
       </c>
@@ -3932,8 +4363,11 @@
       <c r="E131" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="G131" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -3949,8 +4383,11 @@
       <c r="E132" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="G132" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>19</v>
       </c>
@@ -3966,8 +4403,11 @@
       <c r="E133" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="G133" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -3983,8 +4423,11 @@
       <c r="E134" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="G134" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>19</v>
       </c>
@@ -4000,8 +4443,11 @@
       <c r="E135" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="G135" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>19</v>
       </c>
@@ -4017,8 +4463,11 @@
       <c r="E136" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="G136" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>19</v>
       </c>
@@ -4034,8 +4483,11 @@
       <c r="E137" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="G137" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>20</v>
       </c>
@@ -4051,8 +4503,11 @@
       <c r="E138" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="G138" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>20</v>
       </c>
@@ -4068,8 +4523,11 @@
       <c r="E139" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="G139" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>20</v>
       </c>
@@ -4085,8 +4543,11 @@
       <c r="E140" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="G140" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>20</v>
       </c>
@@ -4102,8 +4563,11 @@
       <c r="E141" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="G141" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>20</v>
       </c>
@@ -4119,8 +4583,11 @@
       <c r="E142" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="G142" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>20</v>
       </c>
@@ -4136,8 +4603,11 @@
       <c r="E143" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="G143" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>20</v>
       </c>
@@ -4153,8 +4623,11 @@
       <c r="E144" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="G144" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>20</v>
       </c>
@@ -4170,8 +4643,11 @@
       <c r="E145" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="G145" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>20</v>
       </c>
@@ -4187,8 +4663,11 @@
       <c r="E146" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="G146" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>20</v>
       </c>
@@ -4204,8 +4683,11 @@
       <c r="E147" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="G147" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>20</v>
       </c>
@@ -4221,8 +4703,11 @@
       <c r="E148" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="149" spans="1:5">
+      <c r="G148" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>20</v>
       </c>
@@ -4238,8 +4723,11 @@
       <c r="E149" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="G149" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>20</v>
       </c>
@@ -4255,8 +4743,11 @@
       <c r="E150" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="G150" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>20</v>
       </c>
@@ -4272,8 +4763,11 @@
       <c r="E151" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="152" spans="1:5">
+      <c r="G151" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>21</v>
       </c>
@@ -4289,8 +4783,11 @@
       <c r="E152" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="G152" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>21</v>
       </c>
@@ -4306,8 +4803,11 @@
       <c r="E153" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="G153" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>21</v>
       </c>
@@ -4323,8 +4823,11 @@
       <c r="E154" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="G154" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>21</v>
       </c>
@@ -4340,8 +4843,11 @@
       <c r="E155" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="156" spans="1:5">
+      <c r="G155" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>21</v>
       </c>
@@ -4357,8 +4863,11 @@
       <c r="E156" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="G156" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>21</v>
       </c>
@@ -4374,8 +4883,11 @@
       <c r="E157" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="158" spans="1:5">
+      <c r="G157" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>22</v>
       </c>
@@ -4391,8 +4903,11 @@
       <c r="E158" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="159" spans="1:5">
+      <c r="G158" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>22</v>
       </c>
@@ -4408,8 +4923,11 @@
       <c r="E159" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="160" spans="1:5">
+      <c r="G159" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>22</v>
       </c>
@@ -4425,8 +4943,11 @@
       <c r="E160" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="161" spans="1:5">
+      <c r="G160" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>22</v>
       </c>
@@ -4442,8 +4963,11 @@
       <c r="E161" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="162" spans="1:5">
+      <c r="G161" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>22</v>
       </c>
@@ -4459,8 +4983,11 @@
       <c r="E162" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="163" spans="1:5">
+      <c r="G162" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>22</v>
       </c>
@@ -4476,8 +5003,11 @@
       <c r="E163" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="164" spans="1:5">
+      <c r="G163" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>22</v>
       </c>
@@ -4493,8 +5023,11 @@
       <c r="E164" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="165" spans="1:5">
+      <c r="G164" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>22</v>
       </c>
@@ -4510,8 +5043,11 @@
       <c r="E165" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="166" spans="1:5">
+      <c r="G165" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>22</v>
       </c>
@@ -4527,8 +5063,11 @@
       <c r="E166" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="167" spans="1:5">
+      <c r="G166" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>22</v>
       </c>
@@ -4544,8 +5083,11 @@
       <c r="E167" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="168" spans="1:5">
+      <c r="G167" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>22</v>
       </c>
@@ -4561,8 +5103,11 @@
       <c r="E168" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="169" spans="1:5">
+      <c r="G168" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>22</v>
       </c>
@@ -4578,8 +5123,11 @@
       <c r="E169" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="170" spans="1:5">
+      <c r="G169" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>23</v>
       </c>
@@ -4595,8 +5143,11 @@
       <c r="E170" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="171" spans="1:5">
+      <c r="G170" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>23</v>
       </c>
@@ -4612,8 +5163,11 @@
       <c r="E171" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="172" spans="1:5">
+      <c r="G171" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>23</v>
       </c>
@@ -4629,8 +5183,11 @@
       <c r="E172" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="173" spans="1:5">
+      <c r="G172" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>23</v>
       </c>
@@ -4646,8 +5203,11 @@
       <c r="E173" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="174" spans="1:5">
+      <c r="G173" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>23</v>
       </c>
@@ -4663,8 +5223,11 @@
       <c r="E174" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="175" spans="1:5">
+      <c r="G174" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>23</v>
       </c>
@@ -4680,8 +5243,11 @@
       <c r="E175" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="176" spans="1:5">
+      <c r="G175" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>23</v>
       </c>
@@ -4697,8 +5263,11 @@
       <c r="E176" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="177" spans="1:5">
+      <c r="G176" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>23</v>
       </c>
@@ -4714,8 +5283,11 @@
       <c r="E177" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="178" spans="1:5">
+      <c r="G177" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>23</v>
       </c>
@@ -4731,8 +5303,11 @@
       <c r="E178" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="179" spans="1:5">
+      <c r="G178" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>23</v>
       </c>
@@ -4748,8 +5323,11 @@
       <c r="E179" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="180" spans="1:5">
+      <c r="G179" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>23</v>
       </c>
@@ -4765,8 +5343,11 @@
       <c r="E180" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="181" spans="1:5">
+      <c r="G180" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>23</v>
       </c>
@@ -4782,8 +5363,11 @@
       <c r="E181" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="182" spans="1:5">
+      <c r="G181" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>23</v>
       </c>
@@ -4799,8 +5383,11 @@
       <c r="E182" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="183" spans="1:5">
+      <c r="G182" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>24</v>
       </c>
@@ -4816,8 +5403,11 @@
       <c r="E183" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="184" spans="1:5">
+      <c r="G183" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>24</v>
       </c>
@@ -4833,8 +5423,11 @@
       <c r="E184" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="185" spans="1:5">
+      <c r="G184" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>24</v>
       </c>
@@ -4850,8 +5443,11 @@
       <c r="E185" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="186" spans="1:5">
+      <c r="G185" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>24</v>
       </c>
@@ -4867,8 +5463,11 @@
       <c r="E186" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="187" spans="1:5">
+      <c r="G186" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>24</v>
       </c>
@@ -4884,8 +5483,11 @@
       <c r="E187" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="188" spans="1:5">
+      <c r="G187" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>24</v>
       </c>
@@ -4901,8 +5503,11 @@
       <c r="E188" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="189" spans="1:5">
+      <c r="G188" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>24</v>
       </c>
@@ -4918,8 +5523,11 @@
       <c r="E189" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="190" spans="1:5">
+      <c r="G189" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>24</v>
       </c>
@@ -4935,8 +5543,11 @@
       <c r="E190" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="191" spans="1:5">
+      <c r="G190" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>25</v>
       </c>
@@ -4952,8 +5563,11 @@
       <c r="E191" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="192" spans="1:5">
+      <c r="G191" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>25</v>
       </c>
@@ -4969,8 +5583,11 @@
       <c r="E192" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="193" spans="1:5">
+      <c r="G192" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>25</v>
       </c>
@@ -4986,8 +5603,11 @@
       <c r="E193" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="194" spans="1:5">
+      <c r="G193" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>25</v>
       </c>
@@ -5003,8 +5623,11 @@
       <c r="E194" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="195" spans="1:5">
+      <c r="G194" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>25</v>
       </c>
@@ -5020,8 +5643,11 @@
       <c r="E195" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="196" spans="1:5">
+      <c r="G195" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>25</v>
       </c>
@@ -5037,8 +5663,11 @@
       <c r="E196" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="197" spans="1:5">
+      <c r="G196" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>25</v>
       </c>
@@ -5054,8 +5683,11 @@
       <c r="E197" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="198" spans="1:5">
+      <c r="G197" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>25</v>
       </c>
@@ -5070,6 +5702,9 @@
       </c>
       <c r="E198" t="s">
         <v>440</v>
+      </c>
+      <c r="G198" t="s">
+        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>